<commit_message>
Commit de documentacion para demo
</commit_message>
<xml_diff>
--- a/Documentacion/Planificacion - Gantt 2da Entrega.xlsx
+++ b/Documentacion/Planificacion - Gantt 2da Entrega.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reaperwest\Documents\GitHub\Taller12019\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpouso\Documents\Mathias\Taller 1 2019\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883C4CA8-21E0-45DC-BD03-81A0C5151325}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02437E25-99DD-4923-8923-0DB50AA2C1B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1225,11 +1225,11 @@
   </sheetPr>
   <dimension ref="A1:AS50"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="AU33" sqref="AU33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="40" width="3.125" customWidth="1"/>

</xml_diff>